<commit_message>
Avance: generación boleto pdf
</commit_message>
<xml_diff>
--- a/reports/reporte_ventas.xlsx
+++ b/reports/reporte_ventas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,453 +436,473 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>nro_venta</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>codigo_venta</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>nro_pasaje</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>fecha_venta</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>nombre_vendedor</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>rut_vendedor</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>ciudad_origen</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>ciudad_destino</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>hora_salida</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>hora_llegada</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>patente_bus</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>chofer</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>rut_chofer</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>estado_viaje</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>sub_total</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>iva</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>total</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>codigo_venta</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>7</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>3d372c36-3aa3-44f6-b350-1954d9c43d68</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>2024-12-19</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>Raúl Fernández</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>34567890-1</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>Valparaíso</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>Osorno</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>2024-12-19 12:00:00</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>2024-12-15 22:30:00</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>OPQR12</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>Carlos Fernández</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>23456789-0</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>pendiente</t>
         </is>
-      </c>
-      <c r="M2" t="n">
-        <v>29000</v>
-      </c>
-      <c r="N2" t="n">
-        <v>1.19</v>
       </c>
       <c r="O2" t="n">
         <v>29000</v>
       </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>3d372c36-3aa3-44f6-b350-1954d9c43d68</t>
-        </is>
+      <c r="P2" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>29000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
+        <v>8</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>197e9b3f-441e-46c6-b7a4-517bf46ca013</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>2024-12-18</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Raúl Fernández</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>34567890-1</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>Concepción</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Punta Arenas</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>2024-12-18 08:00:00</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>2024-12-15 14:30:00</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>JKLM78</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>Luis Rodríguez</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>67890123-4</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>pendiente</t>
         </is>
-      </c>
-      <c r="M3" t="n">
-        <v>67000</v>
-      </c>
-      <c r="N3" t="n">
-        <v>1.19</v>
       </c>
       <c r="O3" t="n">
         <v>67000</v>
       </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>197e9b3f-441e-46c6-b7a4-517bf46ca013</t>
-        </is>
+      <c r="P3" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>67000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
+        <v>9</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>086d2f41-0488-47c8-989d-5dad72b93ede</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>2024-12-19</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>Raúl Fernández</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>34567890-1</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>Valparaíso</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>Osorno</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>2024-12-19 13:00:00</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>2024-12-15 23:30:00</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>ABCDE</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>Juanita Díaz</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>12345678-9</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>pendiente</t>
         </is>
-      </c>
-      <c r="M4" t="n">
-        <v>29000</v>
-      </c>
-      <c r="N4" t="n">
-        <v>1.19</v>
       </c>
       <c r="O4" t="n">
         <v>29000</v>
       </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>086d2f41-0488-47c8-989d-5dad72b93ede</t>
-        </is>
+      <c r="P4" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>29000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
+        <v>10</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>d01582e7-ead5-4a36-bb95-cdc416153775</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>2024-12-19</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Raúl Fernández</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>34567890-1</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>Valparaíso</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>Osorno</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>2024-12-19 12:00:00</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>2024-12-15 22:30:00</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>OPQR12</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>Carlos Fernández</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>23456789-0</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>pendiente</t>
         </is>
-      </c>
-      <c r="M5" t="n">
-        <v>29000</v>
-      </c>
-      <c r="N5" t="n">
-        <v>1.19</v>
       </c>
       <c r="O5" t="n">
         <v>29000</v>
       </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>d01582e7-ead5-4a36-bb95-cdc416153775</t>
-        </is>
+      <c r="P5" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>29000</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
+        <v>11</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>81f9c270-66f7-4d3a-9aa5-176ca7e998b8</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
         <v>5</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>2024-12-18</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>Raúl Fernández</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>34567890-1</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>Concepción</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>Punta Arenas</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>2024-12-18 08:00:00</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>2024-12-15 14:30:00</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>JKLM78</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>Luis Rodríguez</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="M6" t="inlineStr">
         <is>
           <t>67890123-4</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="N6" t="inlineStr">
         <is>
           <t>pendiente</t>
         </is>
-      </c>
-      <c r="M6" t="n">
-        <v>67000</v>
-      </c>
-      <c r="N6" t="n">
-        <v>1.19</v>
       </c>
       <c r="O6" t="n">
         <v>67000</v>
       </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>81f9c270-66f7-4d3a-9aa5-176ca7e998b8</t>
-        </is>
+      <c r="P6" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>67000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>